<commit_message>
update time sleep rule
</commit_message>
<xml_diff>
--- a/storage/pa_template/item_template.xlsx
+++ b/storage/pa_template/item_template.xlsx
@@ -22,68 +22,69 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t xml:space="preserve">game</t>
-  </si>
-  <si>
-    <t xml:space="preserve">server</t>
-  </si>
-  <si>
-    <t xml:space="preserve">faction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_category1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_category2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_category3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_per_unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unit_price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min_unit_per_order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">price_currency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ValueForDiscount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">discount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">offer_duration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delivery_guarantee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delivery_info</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cover_image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description</t>
+    <t xml:space="preserve">Game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item Category 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item Category 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item Category 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item Per Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock(Total units)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min. Units Per Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value For Discount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% Discount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offer Duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery Guarantee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cover image (PA hosted)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -108,18 +109,39 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
-      <charset val="1"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000080"/>
+        <bgColor rgb="FF000080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -163,13 +185,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -192,12 +230,12 @@
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O16" activeCellId="0" sqref="O16"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -228,22 +266,22 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
@@ -253,7 +291,26 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+    </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>